<commit_message>
Change memory map Added reverse gait, movement prepare sequence and movement end sequence
</commit_message>
<xml_diff>
--- a/Docs/Memory map.xlsx
+++ b/Docs/Memory map.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RAM0" sheetId="11" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="155">
   <si>
     <t>A</t>
   </si>
@@ -367,77 +367,6 @@
   </si>
   <si>
     <t>servo_ch_15 override</t>
-  </si>
-  <si>
-    <t>Servo_ch_0
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_4
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_8
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_12
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_16
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_2
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_6</t>
-  </si>
-  <si>
-    <t>Servo_ch_10
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_14
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_1
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_5
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_9
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_13
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_15
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_3
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_7
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_11
-zero</t>
-  </si>
-  <si>
-    <t>Servo_ch_17
-zero</t>
   </si>
   <si>
     <t>Servo_ch_x zero</t>
@@ -569,6 +498,81 @@
   </si>
   <si>
     <t>Start position Y</t>
+  </si>
+  <si>
+    <t>Physic
+zero trim 1</t>
+  </si>
+  <si>
+    <t>Physic 
+zero trim 0</t>
+  </si>
+  <si>
+    <t>Physic
+zero trim 2</t>
+  </si>
+  <si>
+    <t>Physic 
+zero trim 4</t>
+  </si>
+  <si>
+    <t>Physic
+zero trim 6</t>
+  </si>
+  <si>
+    <t>Physic 
+zero trim 8</t>
+  </si>
+  <si>
+    <t>Physic
+zero trim 10</t>
+  </si>
+  <si>
+    <t>Physic 
+zero trim 12</t>
+  </si>
+  <si>
+    <t>Physic
+zero trim 14</t>
+  </si>
+  <si>
+    <t>Physic 
+zero trim 16</t>
+  </si>
+  <si>
+    <t>Physic 
+zero trim 3</t>
+  </si>
+  <si>
+    <t>Physic
+zero trim 5</t>
+  </si>
+  <si>
+    <t>Physic 
+zero trim 7</t>
+  </si>
+  <si>
+    <t>Physic
+zero trim 9</t>
+  </si>
+  <si>
+    <t>Physic 
+zero trim 11</t>
+  </si>
+  <si>
+    <t>Physic
+zero trim 13</t>
+  </si>
+  <si>
+    <t>Physic 
+zero trim 15</t>
+  </si>
+  <si>
+    <t>Physic
+zero trim 17</t>
+  </si>
+  <si>
+    <t>Start logical zero</t>
   </si>
 </sst>
 </file>
@@ -1492,56 +1496,146 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1579,16 +1673,22 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1665,102 +1765,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2085,44 +2089,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
+      <c r="B2" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2180,14 +2184,14 @@
       <c r="B6" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
       <c r="G6" s="52" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="H6" s="41"/>
       <c r="I6" s="41"/>
@@ -2591,399 +2595,426 @@
       <c r="R21" s="33"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="O25" s="64"/>
-      <c r="P25" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q25" s="64"/>
-      <c r="R25" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="S25" s="64"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" s="90"/>
+      <c r="P25" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q25" s="90"/>
+      <c r="R25" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="S25" s="90"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="66"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="64"/>
-      <c r="O26" s="64"/>
-      <c r="P26" s="64"/>
-      <c r="Q26" s="64"/>
-      <c r="R26" s="64"/>
-      <c r="S26" s="64"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="90"/>
+      <c r="N26" s="90"/>
+      <c r="O26" s="90"/>
+      <c r="P26" s="90"/>
+      <c r="Q26" s="90"/>
+      <c r="R26" s="90"/>
+      <c r="S26" s="90"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="64"/>
-      <c r="P27" s="64"/>
-      <c r="Q27" s="64"/>
-      <c r="R27" s="64"/>
-      <c r="S27" s="64"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="90"/>
+      <c r="N27" s="90"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="90"/>
+      <c r="Q27" s="90"/>
+      <c r="R27" s="90"/>
+      <c r="S27" s="90"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
-      <c r="O28" s="64"/>
-      <c r="P28" s="64"/>
-      <c r="Q28" s="64"/>
-      <c r="R28" s="64"/>
-      <c r="S28" s="64"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
+      <c r="P28" s="90"/>
+      <c r="Q28" s="90"/>
+      <c r="R28" s="90"/>
+      <c r="S28" s="90"/>
     </row>
     <row r="29" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="66"/>
-      <c r="D29" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="64"/>
-      <c r="F29" s="67" t="s">
-        <v>149</v>
-      </c>
-      <c r="G29" s="68"/>
-      <c r="H29" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="I29" s="68"/>
-      <c r="J29" s="67" t="s">
-        <v>147</v>
-      </c>
-      <c r="K29" s="68"/>
-      <c r="L29" s="67" t="s">
-        <v>146</v>
-      </c>
-      <c r="M29" s="68"/>
-      <c r="N29" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="O29" s="68"/>
-      <c r="P29" s="67" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q29" s="68"/>
-      <c r="R29" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="S29" s="68"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="90"/>
+      <c r="F29" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="92"/>
+      <c r="H29" s="91" t="s">
+        <v>130</v>
+      </c>
+      <c r="I29" s="92"/>
+      <c r="J29" s="91" t="s">
+        <v>129</v>
+      </c>
+      <c r="K29" s="92"/>
+      <c r="L29" s="91" t="s">
+        <v>128</v>
+      </c>
+      <c r="M29" s="92"/>
+      <c r="N29" s="91" t="s">
+        <v>127</v>
+      </c>
+      <c r="O29" s="92"/>
+      <c r="P29" s="91" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q29" s="92"/>
+      <c r="R29" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="S29" s="92"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="70"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="70"/>
-      <c r="N30" s="69"/>
-      <c r="O30" s="70"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="70"/>
-      <c r="R30" s="69"/>
-      <c r="S30" s="70"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="93"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="93"/>
+      <c r="M30" s="94"/>
+      <c r="N30" s="93"/>
+      <c r="O30" s="94"/>
+      <c r="P30" s="93"/>
+      <c r="Q30" s="94"/>
+      <c r="R30" s="93"/>
+      <c r="S30" s="94"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="70"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="70"/>
-      <c r="N31" s="69"/>
-      <c r="O31" s="70"/>
-      <c r="P31" s="69"/>
-      <c r="Q31" s="70"/>
-      <c r="R31" s="69"/>
-      <c r="S31" s="70"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="93"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="93"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="93"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="93"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="93"/>
+      <c r="S31" s="94"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="66"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="71"/>
-      <c r="K32" s="72"/>
-      <c r="L32" s="71"/>
-      <c r="M32" s="72"/>
-      <c r="N32" s="71"/>
-      <c r="O32" s="72"/>
-      <c r="P32" s="71"/>
-      <c r="Q32" s="72"/>
-      <c r="R32" s="71"/>
-      <c r="S32" s="72"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="95"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="95"/>
+      <c r="I32" s="96"/>
+      <c r="J32" s="95"/>
+      <c r="K32" s="96"/>
+      <c r="L32" s="95"/>
+      <c r="M32" s="96"/>
+      <c r="N32" s="95"/>
+      <c r="O32" s="96"/>
+      <c r="P32" s="95"/>
+      <c r="Q32" s="96"/>
+      <c r="R32" s="95"/>
+      <c r="S32" s="96"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="66"/>
-      <c r="D33" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="K33" s="64"/>
-      <c r="L33" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="O33" s="64"/>
-      <c r="P33" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q33" s="64"/>
-      <c r="R33" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="S33" s="64"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="90"/>
+      <c r="H33" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="I33" s="90"/>
+      <c r="J33" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="K33" s="90"/>
+      <c r="L33" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="M33" s="90"/>
+      <c r="N33" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="O33" s="90"/>
+      <c r="P33" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q33" s="90"/>
+      <c r="R33" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="S33" s="90"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="64"/>
-      <c r="N34" s="64"/>
-      <c r="O34" s="64"/>
-      <c r="P34" s="64"/>
-      <c r="Q34" s="64"/>
-      <c r="R34" s="64"/>
-      <c r="S34" s="64"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="H34" s="90"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="90"/>
+      <c r="N34" s="90"/>
+      <c r="O34" s="90"/>
+      <c r="P34" s="90"/>
+      <c r="Q34" s="90"/>
+      <c r="R34" s="90"/>
+      <c r="S34" s="90"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="66"/>
-      <c r="C35" s="66"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
-      <c r="J35" s="64"/>
-      <c r="K35" s="64"/>
-      <c r="L35" s="64"/>
-      <c r="M35" s="64"/>
-      <c r="N35" s="64"/>
-      <c r="O35" s="64"/>
-      <c r="P35" s="64"/>
-      <c r="Q35" s="64"/>
-      <c r="R35" s="64"/>
-      <c r="S35" s="64"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="H35" s="90"/>
+      <c r="I35" s="90"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="90"/>
+      <c r="L35" s="90"/>
+      <c r="M35" s="90"/>
+      <c r="N35" s="90"/>
+      <c r="O35" s="90"/>
+      <c r="P35" s="90"/>
+      <c r="Q35" s="90"/>
+      <c r="R35" s="90"/>
+      <c r="S35" s="90"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B36" s="66"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="64"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="64"/>
-      <c r="N36" s="64"/>
-      <c r="O36" s="64"/>
-      <c r="P36" s="64"/>
-      <c r="Q36" s="64"/>
-      <c r="R36" s="64"/>
-      <c r="S36" s="64"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="90"/>
+      <c r="H36" s="90"/>
+      <c r="I36" s="90"/>
+      <c r="J36" s="90"/>
+      <c r="K36" s="90"/>
+      <c r="L36" s="90"/>
+      <c r="M36" s="90"/>
+      <c r="N36" s="90"/>
+      <c r="O36" s="90"/>
+      <c r="P36" s="90"/>
+      <c r="Q36" s="90"/>
+      <c r="R36" s="90"/>
+      <c r="S36" s="90"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="65" t="s">
+      <c r="B37" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="66"/>
-      <c r="D37" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="64"/>
-      <c r="F37" s="148" t="s">
-        <v>142</v>
-      </c>
-      <c r="G37" s="149"/>
-      <c r="H37" s="148" t="s">
-        <v>141</v>
-      </c>
-      <c r="I37" s="149"/>
-      <c r="J37" s="148" t="s">
-        <v>140</v>
-      </c>
-      <c r="K37" s="149"/>
-      <c r="L37" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="M37" s="61"/>
-      <c r="N37" s="60" t="s">
+      <c r="C37" s="89"/>
+      <c r="D37" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="90"/>
+      <c r="F37" s="99" t="s">
+        <v>124</v>
+      </c>
+      <c r="G37" s="100"/>
+      <c r="H37" s="99" t="s">
+        <v>123</v>
+      </c>
+      <c r="I37" s="100"/>
+      <c r="J37" s="99" t="s">
+        <v>122</v>
+      </c>
+      <c r="K37" s="100"/>
+      <c r="L37" s="97" t="s">
+        <v>120</v>
+      </c>
+      <c r="M37" s="98"/>
+      <c r="N37" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="O37" s="61"/>
-      <c r="P37" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q37" s="61"/>
-      <c r="R37" s="62" t="s">
-        <v>136</v>
-      </c>
-      <c r="S37" s="63"/>
+      <c r="O37" s="98"/>
+      <c r="P37" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q37" s="98"/>
+      <c r="R37" s="101" t="s">
+        <v>118</v>
+      </c>
+      <c r="S37" s="102"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="66"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="149"/>
-      <c r="G38" s="149"/>
-      <c r="H38" s="149"/>
-      <c r="I38" s="149"/>
-      <c r="J38" s="149"/>
-      <c r="K38" s="149"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="61"/>
-      <c r="O38" s="61"/>
-      <c r="P38" s="61"/>
-      <c r="Q38" s="61"/>
-      <c r="R38" s="63"/>
-      <c r="S38" s="63"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="90"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="100"/>
+      <c r="H38" s="100"/>
+      <c r="I38" s="100"/>
+      <c r="J38" s="100"/>
+      <c r="K38" s="100"/>
+      <c r="L38" s="98"/>
+      <c r="M38" s="98"/>
+      <c r="N38" s="98"/>
+      <c r="O38" s="98"/>
+      <c r="P38" s="98"/>
+      <c r="Q38" s="98"/>
+      <c r="R38" s="102"/>
+      <c r="S38" s="102"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="66"/>
-      <c r="C39" s="66"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="149"/>
-      <c r="G39" s="149"/>
-      <c r="H39" s="149"/>
-      <c r="I39" s="149"/>
-      <c r="J39" s="149"/>
-      <c r="K39" s="149"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="61"/>
-      <c r="O39" s="61"/>
-      <c r="P39" s="61"/>
-      <c r="Q39" s="61"/>
-      <c r="R39" s="63"/>
-      <c r="S39" s="63"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="100"/>
+      <c r="G39" s="100"/>
+      <c r="H39" s="100"/>
+      <c r="I39" s="100"/>
+      <c r="J39" s="100"/>
+      <c r="K39" s="100"/>
+      <c r="L39" s="98"/>
+      <c r="M39" s="98"/>
+      <c r="N39" s="98"/>
+      <c r="O39" s="98"/>
+      <c r="P39" s="98"/>
+      <c r="Q39" s="98"/>
+      <c r="R39" s="102"/>
+      <c r="S39" s="102"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B40" s="66"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="149"/>
-      <c r="G40" s="149"/>
-      <c r="H40" s="149"/>
-      <c r="I40" s="149"/>
-      <c r="J40" s="149"/>
-      <c r="K40" s="149"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="61"/>
-      <c r="O40" s="61"/>
-      <c r="P40" s="61"/>
-      <c r="Q40" s="61"/>
-      <c r="R40" s="63"/>
-      <c r="S40" s="63"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
+      <c r="H40" s="100"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="100"/>
+      <c r="K40" s="100"/>
+      <c r="L40" s="98"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="98"/>
+      <c r="O40" s="98"/>
+      <c r="P40" s="98"/>
+      <c r="Q40" s="98"/>
+      <c r="R40" s="102"/>
+      <c r="S40" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B37:C40"/>
+    <mergeCell ref="D37:E40"/>
+    <mergeCell ref="F37:G40"/>
+    <mergeCell ref="H37:I40"/>
+    <mergeCell ref="J37:K40"/>
+    <mergeCell ref="B33:C36"/>
+    <mergeCell ref="D33:E36"/>
+    <mergeCell ref="F33:G36"/>
+    <mergeCell ref="H33:I36"/>
+    <mergeCell ref="J33:K36"/>
+    <mergeCell ref="L29:M32"/>
+    <mergeCell ref="N29:O32"/>
+    <mergeCell ref="P29:Q32"/>
+    <mergeCell ref="R29:S32"/>
+    <mergeCell ref="N37:O40"/>
+    <mergeCell ref="L37:M40"/>
+    <mergeCell ref="L33:M36"/>
+    <mergeCell ref="P37:Q40"/>
+    <mergeCell ref="R37:S40"/>
+    <mergeCell ref="N33:O36"/>
+    <mergeCell ref="P33:Q36"/>
+    <mergeCell ref="R33:S36"/>
+    <mergeCell ref="B29:C32"/>
+    <mergeCell ref="D29:E32"/>
+    <mergeCell ref="F29:G32"/>
+    <mergeCell ref="H29:I32"/>
+    <mergeCell ref="J29:K32"/>
     <mergeCell ref="B2:R3"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="B25:C28"/>
@@ -2995,33 +3026,6 @@
     <mergeCell ref="N25:O28"/>
     <mergeCell ref="P25:Q28"/>
     <mergeCell ref="R25:S28"/>
-    <mergeCell ref="B29:C32"/>
-    <mergeCell ref="D29:E32"/>
-    <mergeCell ref="F29:G32"/>
-    <mergeCell ref="H29:I32"/>
-    <mergeCell ref="J29:K32"/>
-    <mergeCell ref="L29:M32"/>
-    <mergeCell ref="N29:O32"/>
-    <mergeCell ref="P29:Q32"/>
-    <mergeCell ref="R29:S32"/>
-    <mergeCell ref="N37:O40"/>
-    <mergeCell ref="L37:M40"/>
-    <mergeCell ref="B33:C36"/>
-    <mergeCell ref="D33:E36"/>
-    <mergeCell ref="F33:G36"/>
-    <mergeCell ref="H33:I36"/>
-    <mergeCell ref="J33:K36"/>
-    <mergeCell ref="L33:M36"/>
-    <mergeCell ref="B37:C40"/>
-    <mergeCell ref="D37:E40"/>
-    <mergeCell ref="F37:G40"/>
-    <mergeCell ref="H37:I40"/>
-    <mergeCell ref="J37:K40"/>
-    <mergeCell ref="P37:Q40"/>
-    <mergeCell ref="R37:S40"/>
-    <mergeCell ref="N33:O36"/>
-    <mergeCell ref="P33:Q36"/>
-    <mergeCell ref="R33:S36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3044,44 +3048,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
+      <c r="B2" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3487,7 +3491,7 @@
   </sheetPr>
   <dimension ref="B2:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K14" sqref="K14:L14"/>
     </sheetView>
   </sheetViews>
@@ -3498,143 +3502,143 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="73" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
+      <c r="B2" s="85" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="136"/>
-      <c r="C5" s="137">
+      <c r="B5" s="73"/>
+      <c r="C5" s="74">
         <v>0</v>
       </c>
-      <c r="D5" s="138">
+      <c r="D5" s="75">
         <v>1</v>
       </c>
-      <c r="E5" s="138">
+      <c r="E5" s="75">
         <v>2</v>
       </c>
-      <c r="F5" s="138">
+      <c r="F5" s="75">
         <v>3</v>
       </c>
-      <c r="G5" s="138">
+      <c r="G5" s="75">
         <v>4</v>
       </c>
-      <c r="H5" s="138">
+      <c r="H5" s="75">
         <v>5</v>
       </c>
-      <c r="I5" s="138">
-        <v>6</v>
-      </c>
-      <c r="J5" s="138">
+      <c r="I5" s="75">
+        <v>6</v>
+      </c>
+      <c r="J5" s="75">
         <v>7</v>
       </c>
-      <c r="K5" s="138">
+      <c r="K5" s="75">
         <v>8</v>
       </c>
-      <c r="L5" s="138">
+      <c r="L5" s="75">
         <v>9</v>
       </c>
-      <c r="M5" s="138" t="s">
+      <c r="M5" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="138" t="s">
+      <c r="N5" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="138" t="s">
+      <c r="O5" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="138" t="s">
+      <c r="P5" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="138" t="s">
+      <c r="Q5" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="139" t="s">
+      <c r="R5" s="76" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="118" t="s">
+      <c r="B6" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="124" t="s">
+      <c r="C6" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125" t="s">
+      <c r="D6" s="123"/>
+      <c r="E6" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="125"/>
-      <c r="G6" s="125" t="s">
+      <c r="F6" s="123"/>
+      <c r="G6" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="125"/>
-      <c r="I6" s="125" t="s">
+      <c r="H6" s="123"/>
+      <c r="I6" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="125"/>
-      <c r="K6" s="126" t="s">
+      <c r="J6" s="123"/>
+      <c r="K6" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126" t="s">
+      <c r="L6" s="124"/>
+      <c r="M6" s="124" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="126"/>
-      <c r="O6" s="140" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" s="140" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="140" t="s">
-        <v>6</v>
-      </c>
-      <c r="R6" s="141" t="s">
+      <c r="N6" s="124"/>
+      <c r="O6" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="R6" s="78" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="119" t="s">
+      <c r="B7" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="127" t="s">
+      <c r="C7" s="66" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="51" t="s">
@@ -3652,77 +3656,77 @@
       <c r="H7" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="89" t="s">
-        <v>152</v>
-      </c>
-      <c r="J7" s="89"/>
-      <c r="K7" s="89" t="s">
-        <v>153</v>
-      </c>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89" t="s">
-        <v>151</v>
-      </c>
-      <c r="N7" s="89"/>
-      <c r="O7" s="142" t="s">
-        <v>6</v>
-      </c>
-      <c r="P7" s="142" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="142" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" s="143" t="s">
+      <c r="I7" s="104" t="s">
+        <v>134</v>
+      </c>
+      <c r="J7" s="104"/>
+      <c r="K7" s="104" t="s">
+        <v>135</v>
+      </c>
+      <c r="L7" s="104"/>
+      <c r="M7" s="104" t="s">
+        <v>133</v>
+      </c>
+      <c r="N7" s="104"/>
+      <c r="O7" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="80" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="120" t="s">
+      <c r="B8" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="128" t="s">
+      <c r="C8" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76" t="s">
+      <c r="D8" s="103"/>
+      <c r="E8" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76" t="s">
+      <c r="F8" s="103"/>
+      <c r="G8" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76" t="s">
+      <c r="H8" s="103"/>
+      <c r="I8" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="76"/>
-      <c r="K8" s="88" t="s">
+      <c r="J8" s="103"/>
+      <c r="K8" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88" t="s">
+      <c r="L8" s="118"/>
+      <c r="M8" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="88"/>
-      <c r="O8" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="P8" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="R8" s="145" t="s">
+      <c r="N8" s="118"/>
+      <c r="O8" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="R8" s="82" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="120" t="s">
+      <c r="B9" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="129" t="s">
+      <c r="C9" s="67" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="50" t="s">
@@ -3740,77 +3744,77 @@
       <c r="H9" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="76" t="s">
-        <v>152</v>
-      </c>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76" t="s">
-        <v>153</v>
-      </c>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76" t="s">
-        <v>151</v>
-      </c>
-      <c r="N9" s="76"/>
-      <c r="O9" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9" s="145" t="s">
+      <c r="I9" s="103" t="s">
+        <v>134</v>
+      </c>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103" t="s">
+        <v>135</v>
+      </c>
+      <c r="L9" s="103"/>
+      <c r="M9" s="103" t="s">
+        <v>133</v>
+      </c>
+      <c r="N9" s="103"/>
+      <c r="O9" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="82" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="120" t="s">
+      <c r="B10" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="130" t="s">
+      <c r="C10" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89" t="s">
+      <c r="D10" s="104"/>
+      <c r="E10" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89" t="s">
+      <c r="F10" s="104"/>
+      <c r="G10" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89" t="s">
+      <c r="H10" s="104"/>
+      <c r="I10" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="89"/>
-      <c r="K10" s="90" t="s">
+      <c r="J10" s="104"/>
+      <c r="K10" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="90"/>
-      <c r="M10" s="90" t="s">
+      <c r="L10" s="119"/>
+      <c r="M10" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="N10" s="90"/>
-      <c r="O10" s="146" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10" s="146" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q10" s="146" t="s">
-        <v>6</v>
-      </c>
-      <c r="R10" s="147" t="s">
+      <c r="N10" s="119"/>
+      <c r="O10" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" s="84" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="127" t="s">
+      <c r="C11" s="66" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="51" t="s">
@@ -3828,77 +3832,77 @@
       <c r="H11" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="89" t="s">
-        <v>152</v>
-      </c>
-      <c r="J11" s="89"/>
-      <c r="K11" s="89" t="s">
-        <v>153</v>
-      </c>
-      <c r="L11" s="89"/>
-      <c r="M11" s="89" t="s">
-        <v>151</v>
-      </c>
-      <c r="N11" s="89"/>
-      <c r="O11" s="142" t="s">
-        <v>6</v>
-      </c>
-      <c r="P11" s="142" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q11" s="142" t="s">
-        <v>6</v>
-      </c>
-      <c r="R11" s="143" t="s">
+      <c r="I11" s="104" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104" t="s">
+        <v>135</v>
+      </c>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104" t="s">
+        <v>133</v>
+      </c>
+      <c r="N11" s="104"/>
+      <c r="O11" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="80" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="121" t="s">
+      <c r="B12" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="128" t="s">
+      <c r="C12" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76" t="s">
+      <c r="D12" s="103"/>
+      <c r="E12" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76" t="s">
+      <c r="F12" s="103"/>
+      <c r="G12" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76" t="s">
+      <c r="H12" s="103"/>
+      <c r="I12" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="76"/>
-      <c r="K12" s="88" t="s">
+      <c r="J12" s="103"/>
+      <c r="K12" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="88"/>
-      <c r="M12" s="88" t="s">
+      <c r="L12" s="118"/>
+      <c r="M12" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="N12" s="88"/>
-      <c r="O12" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="P12" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q12" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="R12" s="145" t="s">
+      <c r="N12" s="118"/>
+      <c r="O12" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="P12" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" s="82" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="129" t="s">
+      <c r="C13" s="67" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="50" t="s">
@@ -3916,77 +3920,77 @@
       <c r="H13" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="76" t="s">
-        <v>152</v>
-      </c>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76" t="s">
-        <v>153</v>
-      </c>
-      <c r="L13" s="76"/>
-      <c r="M13" s="76" t="s">
-        <v>151</v>
-      </c>
-      <c r="N13" s="76"/>
-      <c r="O13" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="P13" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q13" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="R13" s="145" t="s">
+      <c r="I13" s="103" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" s="103"/>
+      <c r="K13" s="103" t="s">
+        <v>135</v>
+      </c>
+      <c r="L13" s="103"/>
+      <c r="M13" s="103" t="s">
+        <v>133</v>
+      </c>
+      <c r="N13" s="103"/>
+      <c r="O13" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" s="82" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="130" t="s">
+      <c r="C14" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89" t="s">
+      <c r="D14" s="104"/>
+      <c r="E14" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89" t="s">
+      <c r="F14" s="104"/>
+      <c r="G14" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89" t="s">
+      <c r="H14" s="104"/>
+      <c r="I14" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="89"/>
-      <c r="K14" s="90" t="s">
+      <c r="J14" s="104"/>
+      <c r="K14" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90" t="s">
+      <c r="L14" s="119"/>
+      <c r="M14" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="N14" s="90"/>
-      <c r="O14" s="146" t="s">
-        <v>6</v>
-      </c>
-      <c r="P14" s="146" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q14" s="146" t="s">
-        <v>6</v>
-      </c>
-      <c r="R14" s="147" t="s">
+      <c r="N14" s="119"/>
+      <c r="O14" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="P14" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="R14" s="84" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="121" t="s">
+      <c r="B15" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="127" t="s">
+      <c r="C15" s="66" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="51" t="s">
@@ -4004,77 +4008,77 @@
       <c r="H15" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="89" t="s">
-        <v>152</v>
-      </c>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89" t="s">
-        <v>153</v>
-      </c>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89" t="s">
-        <v>151</v>
-      </c>
-      <c r="N15" s="89"/>
-      <c r="O15" s="142" t="s">
-        <v>6</v>
-      </c>
-      <c r="P15" s="142" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q15" s="142" t="s">
-        <v>6</v>
-      </c>
-      <c r="R15" s="143" t="s">
+      <c r="I15" s="104" t="s">
+        <v>134</v>
+      </c>
+      <c r="J15" s="104"/>
+      <c r="K15" s="104" t="s">
+        <v>135</v>
+      </c>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104" t="s">
+        <v>133</v>
+      </c>
+      <c r="N15" s="104"/>
+      <c r="O15" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="P15" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="R15" s="80" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="128" t="s">
+      <c r="C16" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76" t="s">
+      <c r="D16" s="103"/>
+      <c r="E16" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76" t="s">
+      <c r="F16" s="103"/>
+      <c r="G16" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76" t="s">
+      <c r="H16" s="103"/>
+      <c r="I16" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="76"/>
-      <c r="K16" s="88" t="s">
+      <c r="J16" s="103"/>
+      <c r="K16" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88" t="s">
+      <c r="L16" s="118"/>
+      <c r="M16" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="88"/>
-      <c r="O16" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="P16" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q16" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="R16" s="145" t="s">
+      <c r="N16" s="118"/>
+      <c r="O16" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="P16" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="R16" s="82" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="121" t="s">
+      <c r="B17" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="129" t="s">
+      <c r="C17" s="67" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="50" t="s">
@@ -4092,624 +4096,634 @@
       <c r="H17" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="76" t="s">
-        <v>152</v>
-      </c>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76" t="s">
-        <v>153</v>
-      </c>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76" t="s">
-        <v>151</v>
-      </c>
-      <c r="N17" s="76"/>
-      <c r="O17" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="P17" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q17" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="R17" s="145" t="s">
+      <c r="I17" s="103" t="s">
+        <v>134</v>
+      </c>
+      <c r="J17" s="103"/>
+      <c r="K17" s="103" t="s">
+        <v>135</v>
+      </c>
+      <c r="L17" s="103"/>
+      <c r="M17" s="103" t="s">
+        <v>133</v>
+      </c>
+      <c r="N17" s="103"/>
+      <c r="O17" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="P17" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="R17" s="82" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="121" t="s">
+      <c r="B18" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="131"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="123"/>
-      <c r="I18" s="123"/>
-      <c r="J18" s="123"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
       <c r="O18" s="28"/>
-      <c r="P18" s="123"/>
-      <c r="Q18" s="123"/>
-      <c r="R18" s="132"/>
+      <c r="P18" s="65"/>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="69"/>
     </row>
     <row r="19" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="131"/>
+      <c r="C19" s="68"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="123"/>
-      <c r="I19" s="123"/>
-      <c r="J19" s="123"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
       <c r="O19" s="28"/>
-      <c r="P19" s="123"/>
-      <c r="Q19" s="123"/>
-      <c r="R19" s="132"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="65"/>
+      <c r="R19" s="69"/>
     </row>
     <row r="20" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="121" t="s">
+      <c r="B20" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="131"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
-      <c r="H20" s="123"/>
-      <c r="I20" s="123"/>
-      <c r="J20" s="123"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
       <c r="N20" s="28"/>
       <c r="O20" s="28"/>
-      <c r="P20" s="123"/>
-      <c r="Q20" s="123"/>
-      <c r="R20" s="132"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="69"/>
     </row>
     <row r="21" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="133"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="58"/>
       <c r="E21" s="58"/>
       <c r="F21" s="58"/>
       <c r="G21" s="58"/>
-      <c r="H21" s="134"/>
-      <c r="I21" s="134"/>
-      <c r="J21" s="134"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
       <c r="K21" s="58"/>
       <c r="L21" s="58"/>
       <c r="M21" s="58"/>
       <c r="N21" s="58"/>
       <c r="O21" s="58"/>
-      <c r="P21" s="134"/>
-      <c r="Q21" s="134"/>
-      <c r="R21" s="135"/>
+      <c r="P21" s="71"/>
+      <c r="Q21" s="71"/>
+      <c r="R21" s="72"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="91" t="s">
+      <c r="B25" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="80"/>
-      <c r="M25" s="81"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="108"/>
+      <c r="F25" s="108"/>
+      <c r="G25" s="108"/>
+      <c r="H25" s="108"/>
+      <c r="I25" s="108"/>
+      <c r="J25" s="108"/>
+      <c r="K25" s="109"/>
+      <c r="L25" s="110"/>
+      <c r="M25" s="111"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="92"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="82"/>
-      <c r="L26" s="83"/>
-      <c r="M26" s="84"/>
+      <c r="B26" s="106"/>
+      <c r="C26" s="108"/>
+      <c r="D26" s="108"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="108"/>
+      <c r="H26" s="108"/>
+      <c r="I26" s="108"/>
+      <c r="J26" s="108"/>
+      <c r="K26" s="112"/>
+      <c r="L26" s="113"/>
+      <c r="M26" s="114"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="92"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
-      <c r="J27" s="78"/>
-      <c r="K27" s="82"/>
-      <c r="L27" s="83"/>
-      <c r="M27" s="84"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="113"/>
+      <c r="M27" s="114"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="92"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="85"/>
-      <c r="L28" s="86"/>
-      <c r="M28" s="87"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="108"/>
+      <c r="H28" s="108"/>
+      <c r="I28" s="108"/>
+      <c r="J28" s="108"/>
+      <c r="K28" s="115"/>
+      <c r="L28" s="116"/>
+      <c r="M28" s="117"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="91" t="s">
+      <c r="B29" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="79"/>
-      <c r="L29" s="80"/>
-      <c r="M29" s="81"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="108"/>
+      <c r="H29" s="108"/>
+      <c r="I29" s="108"/>
+      <c r="J29" s="108"/>
+      <c r="K29" s="109"/>
+      <c r="L29" s="110"/>
+      <c r="M29" s="111"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="92"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="78"/>
-      <c r="K30" s="82"/>
-      <c r="L30" s="83"/>
-      <c r="M30" s="84"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="108"/>
+      <c r="F30" s="108"/>
+      <c r="G30" s="108"/>
+      <c r="H30" s="108"/>
+      <c r="I30" s="108"/>
+      <c r="J30" s="108"/>
+      <c r="K30" s="112"/>
+      <c r="L30" s="113"/>
+      <c r="M30" s="114"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="92"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="82"/>
-      <c r="L31" s="83"/>
-      <c r="M31" s="84"/>
+      <c r="B31" s="106"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="108"/>
+      <c r="E31" s="108"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="108"/>
+      <c r="H31" s="108"/>
+      <c r="I31" s="108"/>
+      <c r="J31" s="108"/>
+      <c r="K31" s="112"/>
+      <c r="L31" s="113"/>
+      <c r="M31" s="114"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="92"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="78"/>
-      <c r="K32" s="85"/>
-      <c r="L32" s="86"/>
-      <c r="M32" s="87"/>
+      <c r="B32" s="106"/>
+      <c r="C32" s="108"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="108"/>
+      <c r="G32" s="108"/>
+      <c r="H32" s="108"/>
+      <c r="I32" s="108"/>
+      <c r="J32" s="108"/>
+      <c r="K32" s="115"/>
+      <c r="L32" s="116"/>
+      <c r="M32" s="117"/>
     </row>
     <row r="33" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="91" t="s">
+      <c r="B33" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="77" t="s">
+      <c r="C33" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="78"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="78"/>
-      <c r="K33" s="79"/>
-      <c r="L33" s="80"/>
-      <c r="M33" s="81"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="108"/>
+      <c r="G33" s="108"/>
+      <c r="H33" s="108"/>
+      <c r="I33" s="108"/>
+      <c r="J33" s="108"/>
+      <c r="K33" s="109"/>
+      <c r="L33" s="110"/>
+      <c r="M33" s="111"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="92"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="82"/>
-      <c r="L34" s="83"/>
-      <c r="M34" s="84"/>
+      <c r="B34" s="106"/>
+      <c r="C34" s="108"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="108"/>
+      <c r="F34" s="108"/>
+      <c r="G34" s="108"/>
+      <c r="H34" s="108"/>
+      <c r="I34" s="108"/>
+      <c r="J34" s="108"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="113"/>
+      <c r="M34" s="114"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="92"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="82"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="84"/>
+      <c r="B35" s="106"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="108"/>
+      <c r="F35" s="108"/>
+      <c r="G35" s="108"/>
+      <c r="H35" s="108"/>
+      <c r="I35" s="108"/>
+      <c r="J35" s="108"/>
+      <c r="K35" s="112"/>
+      <c r="L35" s="113"/>
+      <c r="M35" s="114"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="92"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
-      <c r="I36" s="78"/>
-      <c r="J36" s="78"/>
-      <c r="K36" s="85"/>
-      <c r="L36" s="86"/>
-      <c r="M36" s="87"/>
+      <c r="B36" s="106"/>
+      <c r="C36" s="108"/>
+      <c r="D36" s="108"/>
+      <c r="E36" s="108"/>
+      <c r="F36" s="108"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="108"/>
+      <c r="I36" s="108"/>
+      <c r="J36" s="108"/>
+      <c r="K36" s="115"/>
+      <c r="L36" s="116"/>
+      <c r="M36" s="117"/>
     </row>
     <row r="37" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="91" t="s">
+      <c r="B37" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="77" t="s">
+      <c r="C37" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="78"/>
-      <c r="J37" s="78"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="80"/>
-      <c r="M37" s="81"/>
+      <c r="D37" s="108"/>
+      <c r="E37" s="108"/>
+      <c r="F37" s="108"/>
+      <c r="G37" s="108"/>
+      <c r="H37" s="108"/>
+      <c r="I37" s="108"/>
+      <c r="J37" s="108"/>
+      <c r="K37" s="109"/>
+      <c r="L37" s="110"/>
+      <c r="M37" s="111"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="92"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="78"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="78"/>
-      <c r="J38" s="78"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="83"/>
-      <c r="M38" s="84"/>
+      <c r="B38" s="106"/>
+      <c r="C38" s="108"/>
+      <c r="D38" s="108"/>
+      <c r="E38" s="108"/>
+      <c r="F38" s="108"/>
+      <c r="G38" s="108"/>
+      <c r="H38" s="108"/>
+      <c r="I38" s="108"/>
+      <c r="J38" s="108"/>
+      <c r="K38" s="112"/>
+      <c r="L38" s="113"/>
+      <c r="M38" s="114"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="92"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="78"/>
-      <c r="I39" s="78"/>
-      <c r="J39" s="78"/>
-      <c r="K39" s="82"/>
-      <c r="L39" s="83"/>
-      <c r="M39" s="84"/>
+      <c r="B39" s="106"/>
+      <c r="C39" s="108"/>
+      <c r="D39" s="108"/>
+      <c r="E39" s="108"/>
+      <c r="F39" s="108"/>
+      <c r="G39" s="108"/>
+      <c r="H39" s="108"/>
+      <c r="I39" s="108"/>
+      <c r="J39" s="108"/>
+      <c r="K39" s="112"/>
+      <c r="L39" s="113"/>
+      <c r="M39" s="114"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="92"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="78"/>
-      <c r="I40" s="78"/>
-      <c r="J40" s="78"/>
-      <c r="K40" s="85"/>
-      <c r="L40" s="86"/>
-      <c r="M40" s="87"/>
+      <c r="B40" s="106"/>
+      <c r="C40" s="108"/>
+      <c r="D40" s="108"/>
+      <c r="E40" s="108"/>
+      <c r="F40" s="108"/>
+      <c r="G40" s="108"/>
+      <c r="H40" s="108"/>
+      <c r="I40" s="108"/>
+      <c r="J40" s="108"/>
+      <c r="K40" s="115"/>
+      <c r="L40" s="116"/>
+      <c r="M40" s="117"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="91" t="s">
+      <c r="B41" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="77" t="s">
+      <c r="C41" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="78"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="79"/>
-      <c r="L41" s="80"/>
-      <c r="M41" s="81"/>
+      <c r="D41" s="108"/>
+      <c r="E41" s="108"/>
+      <c r="F41" s="108"/>
+      <c r="G41" s="108"/>
+      <c r="H41" s="108"/>
+      <c r="I41" s="108"/>
+      <c r="J41" s="108"/>
+      <c r="K41" s="109"/>
+      <c r="L41" s="110"/>
+      <c r="M41" s="111"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="92"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78"/>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="82"/>
-      <c r="L42" s="83"/>
-      <c r="M42" s="84"/>
+      <c r="B42" s="106"/>
+      <c r="C42" s="108"/>
+      <c r="D42" s="108"/>
+      <c r="E42" s="108"/>
+      <c r="F42" s="108"/>
+      <c r="G42" s="108"/>
+      <c r="H42" s="108"/>
+      <c r="I42" s="108"/>
+      <c r="J42" s="108"/>
+      <c r="K42" s="112"/>
+      <c r="L42" s="113"/>
+      <c r="M42" s="114"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="92"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="78"/>
-      <c r="H43" s="78"/>
-      <c r="I43" s="78"/>
-      <c r="J43" s="78"/>
-      <c r="K43" s="82"/>
-      <c r="L43" s="83"/>
-      <c r="M43" s="84"/>
+      <c r="B43" s="106"/>
+      <c r="C43" s="108"/>
+      <c r="D43" s="108"/>
+      <c r="E43" s="108"/>
+      <c r="F43" s="108"/>
+      <c r="G43" s="108"/>
+      <c r="H43" s="108"/>
+      <c r="I43" s="108"/>
+      <c r="J43" s="108"/>
+      <c r="K43" s="112"/>
+      <c r="L43" s="113"/>
+      <c r="M43" s="114"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="92"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="85"/>
-      <c r="L44" s="86"/>
-      <c r="M44" s="87"/>
+      <c r="B44" s="106"/>
+      <c r="C44" s="108"/>
+      <c r="D44" s="108"/>
+      <c r="E44" s="108"/>
+      <c r="F44" s="108"/>
+      <c r="G44" s="108"/>
+      <c r="H44" s="108"/>
+      <c r="I44" s="108"/>
+      <c r="J44" s="108"/>
+      <c r="K44" s="115"/>
+      <c r="L44" s="116"/>
+      <c r="M44" s="117"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="91" t="s">
+      <c r="B45" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="77" t="s">
+      <c r="C45" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="78"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="78"/>
-      <c r="H45" s="78"/>
-      <c r="I45" s="78"/>
-      <c r="J45" s="78"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="80"/>
-      <c r="M45" s="81"/>
+      <c r="D45" s="108"/>
+      <c r="E45" s="108"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="108"/>
+      <c r="H45" s="108"/>
+      <c r="I45" s="108"/>
+      <c r="J45" s="108"/>
+      <c r="K45" s="109"/>
+      <c r="L45" s="110"/>
+      <c r="M45" s="111"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="92"/>
-      <c r="C46" s="78"/>
-      <c r="D46" s="78"/>
-      <c r="E46" s="78"/>
-      <c r="F46" s="78"/>
-      <c r="G46" s="78"/>
-      <c r="H46" s="78"/>
-      <c r="I46" s="78"/>
-      <c r="J46" s="78"/>
-      <c r="K46" s="82"/>
-      <c r="L46" s="83"/>
-      <c r="M46" s="84"/>
+      <c r="B46" s="106"/>
+      <c r="C46" s="108"/>
+      <c r="D46" s="108"/>
+      <c r="E46" s="108"/>
+      <c r="F46" s="108"/>
+      <c r="G46" s="108"/>
+      <c r="H46" s="108"/>
+      <c r="I46" s="108"/>
+      <c r="J46" s="108"/>
+      <c r="K46" s="112"/>
+      <c r="L46" s="113"/>
+      <c r="M46" s="114"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="92"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="78"/>
-      <c r="G47" s="78"/>
-      <c r="H47" s="78"/>
-      <c r="I47" s="78"/>
-      <c r="J47" s="78"/>
-      <c r="K47" s="82"/>
-      <c r="L47" s="83"/>
-      <c r="M47" s="84"/>
+      <c r="B47" s="106"/>
+      <c r="C47" s="108"/>
+      <c r="D47" s="108"/>
+      <c r="E47" s="108"/>
+      <c r="F47" s="108"/>
+      <c r="G47" s="108"/>
+      <c r="H47" s="108"/>
+      <c r="I47" s="108"/>
+      <c r="J47" s="108"/>
+      <c r="K47" s="112"/>
+      <c r="L47" s="113"/>
+      <c r="M47" s="114"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="92"/>
-      <c r="C48" s="78"/>
-      <c r="D48" s="78"/>
-      <c r="E48" s="78"/>
-      <c r="F48" s="78"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="78"/>
-      <c r="I48" s="78"/>
-      <c r="J48" s="78"/>
-      <c r="K48" s="85"/>
-      <c r="L48" s="86"/>
-      <c r="M48" s="87"/>
+      <c r="B48" s="106"/>
+      <c r="C48" s="108"/>
+      <c r="D48" s="108"/>
+      <c r="E48" s="108"/>
+      <c r="F48" s="108"/>
+      <c r="G48" s="108"/>
+      <c r="H48" s="108"/>
+      <c r="I48" s="108"/>
+      <c r="J48" s="108"/>
+      <c r="K48" s="115"/>
+      <c r="L48" s="116"/>
+      <c r="M48" s="117"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="91" t="s">
+      <c r="B49" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="77" t="s">
+      <c r="C49" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="D49" s="78"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="78"/>
-      <c r="G49" s="78"/>
-      <c r="H49" s="78"/>
-      <c r="I49" s="78"/>
-      <c r="J49" s="78"/>
-      <c r="K49" s="79"/>
-      <c r="L49" s="80"/>
-      <c r="M49" s="81"/>
+      <c r="D49" s="108"/>
+      <c r="E49" s="108"/>
+      <c r="F49" s="108"/>
+      <c r="G49" s="108"/>
+      <c r="H49" s="108"/>
+      <c r="I49" s="108"/>
+      <c r="J49" s="108"/>
+      <c r="K49" s="109"/>
+      <c r="L49" s="110"/>
+      <c r="M49" s="111"/>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="92"/>
-      <c r="C50" s="78"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="78"/>
-      <c r="G50" s="78"/>
-      <c r="H50" s="78"/>
-      <c r="I50" s="78"/>
-      <c r="J50" s="78"/>
-      <c r="K50" s="82"/>
-      <c r="L50" s="83"/>
-      <c r="M50" s="84"/>
+      <c r="B50" s="106"/>
+      <c r="C50" s="108"/>
+      <c r="D50" s="108"/>
+      <c r="E50" s="108"/>
+      <c r="F50" s="108"/>
+      <c r="G50" s="108"/>
+      <c r="H50" s="108"/>
+      <c r="I50" s="108"/>
+      <c r="J50" s="108"/>
+      <c r="K50" s="112"/>
+      <c r="L50" s="113"/>
+      <c r="M50" s="114"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="92"/>
-      <c r="C51" s="78"/>
-      <c r="D51" s="78"/>
-      <c r="E51" s="78"/>
-      <c r="F51" s="78"/>
-      <c r="G51" s="78"/>
-      <c r="H51" s="78"/>
-      <c r="I51" s="78"/>
-      <c r="J51" s="78"/>
-      <c r="K51" s="82"/>
-      <c r="L51" s="83"/>
-      <c r="M51" s="84"/>
+      <c r="B51" s="106"/>
+      <c r="C51" s="108"/>
+      <c r="D51" s="108"/>
+      <c r="E51" s="108"/>
+      <c r="F51" s="108"/>
+      <c r="G51" s="108"/>
+      <c r="H51" s="108"/>
+      <c r="I51" s="108"/>
+      <c r="J51" s="108"/>
+      <c r="K51" s="112"/>
+      <c r="L51" s="113"/>
+      <c r="M51" s="114"/>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="92"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="78"/>
-      <c r="E52" s="78"/>
-      <c r="F52" s="78"/>
-      <c r="G52" s="78"/>
-      <c r="H52" s="78"/>
-      <c r="I52" s="78"/>
-      <c r="J52" s="78"/>
-      <c r="K52" s="85"/>
-      <c r="L52" s="86"/>
-      <c r="M52" s="87"/>
+      <c r="B52" s="106"/>
+      <c r="C52" s="108"/>
+      <c r="D52" s="108"/>
+      <c r="E52" s="108"/>
+      <c r="F52" s="108"/>
+      <c r="G52" s="108"/>
+      <c r="H52" s="108"/>
+      <c r="I52" s="108"/>
+      <c r="J52" s="108"/>
+      <c r="K52" s="115"/>
+      <c r="L52" s="116"/>
+      <c r="M52" s="117"/>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B53" s="91" t="s">
+      <c r="B53" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="77" t="s">
+      <c r="C53" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="D53" s="78"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="78"/>
-      <c r="G53" s="78"/>
-      <c r="H53" s="78"/>
-      <c r="I53" s="78"/>
-      <c r="J53" s="78"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="80"/>
-      <c r="M53" s="81"/>
+      <c r="D53" s="108"/>
+      <c r="E53" s="108"/>
+      <c r="F53" s="108"/>
+      <c r="G53" s="108"/>
+      <c r="H53" s="108"/>
+      <c r="I53" s="108"/>
+      <c r="J53" s="108"/>
+      <c r="K53" s="109"/>
+      <c r="L53" s="110"/>
+      <c r="M53" s="111"/>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B54" s="92"/>
-      <c r="C54" s="78"/>
-      <c r="D54" s="78"/>
-      <c r="E54" s="78"/>
-      <c r="F54" s="78"/>
-      <c r="G54" s="78"/>
-      <c r="H54" s="78"/>
-      <c r="I54" s="78"/>
-      <c r="J54" s="78"/>
-      <c r="K54" s="82"/>
-      <c r="L54" s="83"/>
-      <c r="M54" s="84"/>
+      <c r="B54" s="106"/>
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="108"/>
+      <c r="F54" s="108"/>
+      <c r="G54" s="108"/>
+      <c r="H54" s="108"/>
+      <c r="I54" s="108"/>
+      <c r="J54" s="108"/>
+      <c r="K54" s="112"/>
+      <c r="L54" s="113"/>
+      <c r="M54" s="114"/>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B55" s="92"/>
-      <c r="C55" s="78"/>
-      <c r="D55" s="78"/>
-      <c r="E55" s="78"/>
-      <c r="F55" s="78"/>
-      <c r="G55" s="78"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="78"/>
-      <c r="J55" s="78"/>
-      <c r="K55" s="82"/>
-      <c r="L55" s="83"/>
-      <c r="M55" s="84"/>
+      <c r="B55" s="106"/>
+      <c r="C55" s="108"/>
+      <c r="D55" s="108"/>
+      <c r="E55" s="108"/>
+      <c r="F55" s="108"/>
+      <c r="G55" s="108"/>
+      <c r="H55" s="108"/>
+      <c r="I55" s="108"/>
+      <c r="J55" s="108"/>
+      <c r="K55" s="112"/>
+      <c r="L55" s="113"/>
+      <c r="M55" s="114"/>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B56" s="92"/>
-      <c r="C56" s="78"/>
-      <c r="D56" s="78"/>
-      <c r="E56" s="78"/>
-      <c r="F56" s="78"/>
-      <c r="G56" s="78"/>
-      <c r="H56" s="78"/>
-      <c r="I56" s="78"/>
-      <c r="J56" s="78"/>
-      <c r="K56" s="85"/>
-      <c r="L56" s="86"/>
-      <c r="M56" s="87"/>
+      <c r="B56" s="106"/>
+      <c r="C56" s="108"/>
+      <c r="D56" s="108"/>
+      <c r="E56" s="108"/>
+      <c r="F56" s="108"/>
+      <c r="G56" s="108"/>
+      <c r="H56" s="108"/>
+      <c r="I56" s="108"/>
+      <c r="J56" s="108"/>
+      <c r="K56" s="115"/>
+      <c r="L56" s="116"/>
+      <c r="M56" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="C49:J52"/>
-    <mergeCell ref="K49:M52"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="C53:J56"/>
-    <mergeCell ref="K53:M56"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C41:J44"/>
-    <mergeCell ref="K41:M44"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="C45:J48"/>
-    <mergeCell ref="K45:M48"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C25:J28"/>
+    <mergeCell ref="K25:M28"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="C37:J40"/>
     <mergeCell ref="K37:M40"/>
@@ -4723,45 +4737,35 @@
     <mergeCell ref="B29:B32"/>
     <mergeCell ref="C29:J32"/>
     <mergeCell ref="K29:M32"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C41:J44"/>
+    <mergeCell ref="K41:M44"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="C45:J48"/>
+    <mergeCell ref="K45:M48"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="C49:J52"/>
+    <mergeCell ref="K49:M52"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="C53:J56"/>
+    <mergeCell ref="K53:M56"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C25:J28"/>
-    <mergeCell ref="K25:M28"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4775,9 +4779,7 @@
   </sheetPr>
   <dimension ref="B2:S38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:S34"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4786,44 +4788,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
+      <c r="B2" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4881,17 +4883,17 @@
       <c r="B6" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>108</v>
+      <c r="C6" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>129</v>
+      <c r="E6" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>6</v>
@@ -4905,17 +4907,17 @@
       <c r="J6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>117</v>
+      <c r="K6" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="18" t="s">
-        <v>129</v>
+      <c r="M6" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="N6" s="18" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>6</v>
@@ -4934,17 +4936,17 @@
       <c r="B7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>113</v>
+      <c r="C7" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>129</v>
+      <c r="E7" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>6</v>
@@ -4958,17 +4960,17 @@
       <c r="J7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>122</v>
+      <c r="K7" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="7" t="s">
-        <v>129</v>
+      <c r="M7" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>6</v>
@@ -4987,17 +4989,17 @@
       <c r="B8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>109</v>
+      <c r="C8" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>129</v>
+      <c r="E8" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>6</v>
@@ -5011,19 +5013,19 @@
       <c r="J8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>118</v>
+      <c r="K8" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="L8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="18" t="s">
-        <v>129</v>
+      <c r="M8" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="N8" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="O8" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="O8" s="19" t="s">
         <v>6</v>
       </c>
       <c r="P8" s="19" t="s">
@@ -5040,19 +5042,19 @@
       <c r="B9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>114</v>
+      <c r="C9" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>129</v>
+      <c r="E9" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="G9" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" s="19" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="19" t="s">
@@ -5064,17 +5066,17 @@
       <c r="J9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>123</v>
+      <c r="K9" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="7" t="s">
-        <v>129</v>
+      <c r="M9" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>6</v>
@@ -5093,17 +5095,17 @@
       <c r="B10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>110</v>
+      <c r="C10" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>129</v>
+      <c r="E10" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>6</v>
@@ -5117,19 +5119,19 @@
       <c r="J10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>119</v>
+      <c r="K10" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="L10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="18" t="s">
-        <v>129</v>
+      <c r="M10" s="17" t="s">
+        <v>149</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="O10" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="O10" s="19" t="s">
         <v>6</v>
       </c>
       <c r="P10" s="19" t="s">
@@ -5146,19 +5148,19 @@
       <c r="B11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>115</v>
+      <c r="C11" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>129</v>
+      <c r="E11" s="17" t="s">
+        <v>142</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="G11" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>6</v>
       </c>
       <c r="H11" s="19" t="s">
@@ -5170,17 +5172,17 @@
       <c r="J11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>124</v>
+      <c r="K11" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="7" t="s">
-        <v>129</v>
+      <c r="M11" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>6</v>
@@ -5199,17 +5201,17 @@
       <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>111</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>129</v>
+      <c r="E12" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>6</v>
@@ -5223,19 +5225,19 @@
       <c r="J12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="17" t="s">
-        <v>120</v>
+      <c r="K12" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="L12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="18" t="s">
-        <v>129</v>
+      <c r="M12" s="17" t="s">
+        <v>151</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="O12" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="O12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="P12" s="19" t="s">
@@ -5252,19 +5254,19 @@
       <c r="B13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>116</v>
+      <c r="C13" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>129</v>
+      <c r="E13" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="19" t="s">
@@ -5276,17 +5278,17 @@
       <c r="J13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>121</v>
+      <c r="K13" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="7" t="s">
-        <v>129</v>
+      <c r="M13" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>6</v>
@@ -5305,17 +5307,17 @@
       <c r="B14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>112</v>
+      <c r="C14" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>129</v>
+      <c r="E14" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>6</v>
@@ -5329,19 +5331,19 @@
       <c r="J14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="17" t="s">
-        <v>125</v>
+      <c r="K14" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="L14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="18" t="s">
-        <v>129</v>
+      <c r="M14" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="N14" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="O14" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="O14" s="19" t="s">
         <v>6</v>
       </c>
       <c r="P14" s="19" t="s">
@@ -5502,340 +5504,340 @@
       <c r="R21" s="33"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="93" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="94"/>
-      <c r="D23" s="95" t="s">
-        <v>139</v>
-      </c>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
-      <c r="K23" s="110"/>
-      <c r="L23" s="110"/>
-      <c r="M23" s="110"/>
-      <c r="N23" s="110"/>
-      <c r="O23" s="110"/>
-      <c r="P23" s="110"/>
-      <c r="Q23" s="110"/>
-      <c r="R23" s="110"/>
-      <c r="S23" s="111"/>
+      <c r="B23" s="125" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="126"/>
+      <c r="D23" s="127" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="142"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="142"/>
+      <c r="I23" s="142"/>
+      <c r="J23" s="142"/>
+      <c r="K23" s="142"/>
+      <c r="L23" s="142"/>
+      <c r="M23" s="142"/>
+      <c r="N23" s="142"/>
+      <c r="O23" s="142"/>
+      <c r="P23" s="142"/>
+      <c r="Q23" s="142"/>
+      <c r="R23" s="142"/>
+      <c r="S23" s="143"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="94"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="113"/>
-      <c r="G24" s="113"/>
-      <c r="H24" s="113"/>
-      <c r="I24" s="113"/>
-      <c r="J24" s="113"/>
-      <c r="K24" s="113"/>
-      <c r="L24" s="113"/>
-      <c r="M24" s="113"/>
-      <c r="N24" s="113"/>
-      <c r="O24" s="113"/>
-      <c r="P24" s="113"/>
-      <c r="Q24" s="113"/>
-      <c r="R24" s="113"/>
-      <c r="S24" s="114"/>
+      <c r="B24" s="126"/>
+      <c r="C24" s="126"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="145"/>
+      <c r="F24" s="145"/>
+      <c r="G24" s="145"/>
+      <c r="H24" s="145"/>
+      <c r="I24" s="145"/>
+      <c r="J24" s="145"/>
+      <c r="K24" s="145"/>
+      <c r="L24" s="145"/>
+      <c r="M24" s="145"/>
+      <c r="N24" s="145"/>
+      <c r="O24" s="145"/>
+      <c r="P24" s="145"/>
+      <c r="Q24" s="145"/>
+      <c r="R24" s="145"/>
+      <c r="S24" s="146"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="94"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="113"/>
-      <c r="G25" s="113"/>
-      <c r="H25" s="113"/>
-      <c r="I25" s="113"/>
-      <c r="J25" s="113"/>
-      <c r="K25" s="113"/>
-      <c r="L25" s="113"/>
-      <c r="M25" s="113"/>
-      <c r="N25" s="113"/>
-      <c r="O25" s="113"/>
-      <c r="P25" s="113"/>
-      <c r="Q25" s="113"/>
-      <c r="R25" s="113"/>
-      <c r="S25" s="114"/>
+      <c r="B25" s="126"/>
+      <c r="C25" s="126"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
+      <c r="K25" s="145"/>
+      <c r="L25" s="145"/>
+      <c r="M25" s="145"/>
+      <c r="N25" s="145"/>
+      <c r="O25" s="145"/>
+      <c r="P25" s="145"/>
+      <c r="Q25" s="145"/>
+      <c r="R25" s="145"/>
+      <c r="S25" s="146"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="94"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="115"/>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="116"/>
-      <c r="J26" s="116"/>
-      <c r="K26" s="116"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="116"/>
-      <c r="N26" s="116"/>
-      <c r="O26" s="116"/>
-      <c r="P26" s="116"/>
-      <c r="Q26" s="116"/>
-      <c r="R26" s="116"/>
-      <c r="S26" s="117"/>
+      <c r="B26" s="126"/>
+      <c r="C26" s="126"/>
+      <c r="D26" s="147"/>
+      <c r="E26" s="148"/>
+      <c r="F26" s="148"/>
+      <c r="G26" s="148"/>
+      <c r="H26" s="148"/>
+      <c r="I26" s="148"/>
+      <c r="J26" s="148"/>
+      <c r="K26" s="148"/>
+      <c r="L26" s="148"/>
+      <c r="M26" s="148"/>
+      <c r="N26" s="148"/>
+      <c r="O26" s="148"/>
+      <c r="P26" s="148"/>
+      <c r="Q26" s="148"/>
+      <c r="R26" s="148"/>
+      <c r="S26" s="149"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="94"/>
-      <c r="D27" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="E27" s="96"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="96"/>
-      <c r="H27" s="96"/>
-      <c r="I27" s="96"/>
-      <c r="J27" s="96"/>
-      <c r="K27" s="96"/>
-      <c r="L27" s="96"/>
-      <c r="M27" s="96"/>
-      <c r="N27" s="96"/>
-      <c r="O27" s="96"/>
-      <c r="P27" s="96"/>
-      <c r="Q27" s="96"/>
-      <c r="R27" s="96"/>
-      <c r="S27" s="97"/>
+      <c r="C27" s="126"/>
+      <c r="D27" s="127" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="128"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="128"/>
+      <c r="N27" s="128"/>
+      <c r="O27" s="128"/>
+      <c r="P27" s="128"/>
+      <c r="Q27" s="128"/>
+      <c r="R27" s="128"/>
+      <c r="S27" s="129"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="94"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="99"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="99"/>
-      <c r="J28" s="99"/>
-      <c r="K28" s="99"/>
-      <c r="L28" s="99"/>
-      <c r="M28" s="99"/>
-      <c r="N28" s="99"/>
-      <c r="O28" s="99"/>
-      <c r="P28" s="99"/>
-      <c r="Q28" s="99"/>
-      <c r="R28" s="99"/>
-      <c r="S28" s="100"/>
+      <c r="B28" s="126"/>
+      <c r="C28" s="126"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="131"/>
+      <c r="F28" s="131"/>
+      <c r="G28" s="131"/>
+      <c r="H28" s="131"/>
+      <c r="I28" s="131"/>
+      <c r="J28" s="131"/>
+      <c r="K28" s="131"/>
+      <c r="L28" s="131"/>
+      <c r="M28" s="131"/>
+      <c r="N28" s="131"/>
+      <c r="O28" s="131"/>
+      <c r="P28" s="131"/>
+      <c r="Q28" s="131"/>
+      <c r="R28" s="131"/>
+      <c r="S28" s="132"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="94"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="99"/>
-      <c r="M29" s="99"/>
-      <c r="N29" s="99"/>
-      <c r="O29" s="99"/>
-      <c r="P29" s="99"/>
-      <c r="Q29" s="99"/>
-      <c r="R29" s="99"/>
-      <c r="S29" s="100"/>
+      <c r="B29" s="126"/>
+      <c r="C29" s="126"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="131"/>
+      <c r="F29" s="131"/>
+      <c r="G29" s="131"/>
+      <c r="H29" s="131"/>
+      <c r="I29" s="131"/>
+      <c r="J29" s="131"/>
+      <c r="K29" s="131"/>
+      <c r="L29" s="131"/>
+      <c r="M29" s="131"/>
+      <c r="N29" s="131"/>
+      <c r="O29" s="131"/>
+      <c r="P29" s="131"/>
+      <c r="Q29" s="131"/>
+      <c r="R29" s="131"/>
+      <c r="S29" s="132"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="94"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="102"/>
-      <c r="F30" s="102"/>
-      <c r="G30" s="102"/>
-      <c r="H30" s="102"/>
-      <c r="I30" s="102"/>
-      <c r="J30" s="102"/>
-      <c r="K30" s="102"/>
-      <c r="L30" s="102"/>
-      <c r="M30" s="102"/>
-      <c r="N30" s="102"/>
-      <c r="O30" s="102"/>
-      <c r="P30" s="102"/>
-      <c r="Q30" s="102"/>
-      <c r="R30" s="102"/>
-      <c r="S30" s="103"/>
+      <c r="B30" s="126"/>
+      <c r="C30" s="126"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="134"/>
+      <c r="G30" s="134"/>
+      <c r="H30" s="134"/>
+      <c r="I30" s="134"/>
+      <c r="J30" s="134"/>
+      <c r="K30" s="134"/>
+      <c r="L30" s="134"/>
+      <c r="M30" s="134"/>
+      <c r="N30" s="134"/>
+      <c r="O30" s="134"/>
+      <c r="P30" s="134"/>
+      <c r="Q30" s="134"/>
+      <c r="R30" s="134"/>
+      <c r="S30" s="135"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="104" t="s">
-        <v>129</v>
-      </c>
-      <c r="C31" s="105"/>
-      <c r="D31" s="95" t="s">
-        <v>131</v>
-      </c>
-      <c r="E31" s="96"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="96"/>
-      <c r="I31" s="96"/>
-      <c r="J31" s="96"/>
-      <c r="K31" s="96"/>
-      <c r="L31" s="96"/>
-      <c r="M31" s="96"/>
-      <c r="N31" s="96"/>
-      <c r="O31" s="96"/>
-      <c r="P31" s="96"/>
-      <c r="Q31" s="96"/>
-      <c r="R31" s="96"/>
-      <c r="S31" s="97"/>
+      <c r="B31" s="136" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="137"/>
+      <c r="D31" s="127" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="128"/>
+      <c r="F31" s="128"/>
+      <c r="G31" s="128"/>
+      <c r="H31" s="128"/>
+      <c r="I31" s="128"/>
+      <c r="J31" s="128"/>
+      <c r="K31" s="128"/>
+      <c r="L31" s="128"/>
+      <c r="M31" s="128"/>
+      <c r="N31" s="128"/>
+      <c r="O31" s="128"/>
+      <c r="P31" s="128"/>
+      <c r="Q31" s="128"/>
+      <c r="R31" s="128"/>
+      <c r="S31" s="129"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="106"/>
-      <c r="C32" s="107"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="99"/>
-      <c r="F32" s="99"/>
-      <c r="G32" s="99"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="99"/>
-      <c r="J32" s="99"/>
-      <c r="K32" s="99"/>
-      <c r="L32" s="99"/>
-      <c r="M32" s="99"/>
-      <c r="N32" s="99"/>
-      <c r="O32" s="99"/>
-      <c r="P32" s="99"/>
-      <c r="Q32" s="99"/>
-      <c r="R32" s="99"/>
-      <c r="S32" s="100"/>
+      <c r="B32" s="138"/>
+      <c r="C32" s="139"/>
+      <c r="D32" s="130"/>
+      <c r="E32" s="131"/>
+      <c r="F32" s="131"/>
+      <c r="G32" s="131"/>
+      <c r="H32" s="131"/>
+      <c r="I32" s="131"/>
+      <c r="J32" s="131"/>
+      <c r="K32" s="131"/>
+      <c r="L32" s="131"/>
+      <c r="M32" s="131"/>
+      <c r="N32" s="131"/>
+      <c r="O32" s="131"/>
+      <c r="P32" s="131"/>
+      <c r="Q32" s="131"/>
+      <c r="R32" s="131"/>
+      <c r="S32" s="132"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="106"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="98"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="99"/>
-      <c r="K33" s="99"/>
-      <c r="L33" s="99"/>
-      <c r="M33" s="99"/>
-      <c r="N33" s="99"/>
-      <c r="O33" s="99"/>
-      <c r="P33" s="99"/>
-      <c r="Q33" s="99"/>
-      <c r="R33" s="99"/>
-      <c r="S33" s="100"/>
+      <c r="B33" s="138"/>
+      <c r="C33" s="139"/>
+      <c r="D33" s="130"/>
+      <c r="E33" s="131"/>
+      <c r="F33" s="131"/>
+      <c r="G33" s="131"/>
+      <c r="H33" s="131"/>
+      <c r="I33" s="131"/>
+      <c r="J33" s="131"/>
+      <c r="K33" s="131"/>
+      <c r="L33" s="131"/>
+      <c r="M33" s="131"/>
+      <c r="N33" s="131"/>
+      <c r="O33" s="131"/>
+      <c r="P33" s="131"/>
+      <c r="Q33" s="131"/>
+      <c r="R33" s="131"/>
+      <c r="S33" s="132"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="108"/>
-      <c r="C34" s="109"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="102"/>
-      <c r="F34" s="102"/>
-      <c r="G34" s="102"/>
-      <c r="H34" s="102"/>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
-      <c r="K34" s="102"/>
-      <c r="L34" s="102"/>
-      <c r="M34" s="102"/>
-      <c r="N34" s="102"/>
-      <c r="O34" s="102"/>
-      <c r="P34" s="102"/>
-      <c r="Q34" s="102"/>
-      <c r="R34" s="102"/>
-      <c r="S34" s="103"/>
+      <c r="B34" s="140"/>
+      <c r="C34" s="141"/>
+      <c r="D34" s="133"/>
+      <c r="E34" s="134"/>
+      <c r="F34" s="134"/>
+      <c r="G34" s="134"/>
+      <c r="H34" s="134"/>
+      <c r="I34" s="134"/>
+      <c r="J34" s="134"/>
+      <c r="K34" s="134"/>
+      <c r="L34" s="134"/>
+      <c r="M34" s="134"/>
+      <c r="N34" s="134"/>
+      <c r="O34" s="134"/>
+      <c r="P34" s="134"/>
+      <c r="Q34" s="134"/>
+      <c r="R34" s="134"/>
+      <c r="S34" s="135"/>
     </row>
     <row r="35" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="104" t="s">
-        <v>127</v>
-      </c>
-      <c r="C35" s="105"/>
-      <c r="D35" s="95" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="96"/>
-      <c r="I35" s="96"/>
-      <c r="J35" s="96"/>
-      <c r="K35" s="96"/>
-      <c r="L35" s="96"/>
-      <c r="M35" s="96"/>
-      <c r="N35" s="96"/>
-      <c r="O35" s="96"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="96"/>
-      <c r="R35" s="96"/>
-      <c r="S35" s="97"/>
+      <c r="B35" s="136" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="137"/>
+      <c r="D35" s="127" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="128"/>
+      <c r="F35" s="128"/>
+      <c r="G35" s="128"/>
+      <c r="H35" s="128"/>
+      <c r="I35" s="128"/>
+      <c r="J35" s="128"/>
+      <c r="K35" s="128"/>
+      <c r="L35" s="128"/>
+      <c r="M35" s="128"/>
+      <c r="N35" s="128"/>
+      <c r="O35" s="128"/>
+      <c r="P35" s="128"/>
+      <c r="Q35" s="128"/>
+      <c r="R35" s="128"/>
+      <c r="S35" s="129"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B36" s="106"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
-      <c r="K36" s="99"/>
-      <c r="L36" s="99"/>
-      <c r="M36" s="99"/>
-      <c r="N36" s="99"/>
-      <c r="O36" s="99"/>
-      <c r="P36" s="99"/>
-      <c r="Q36" s="99"/>
-      <c r="R36" s="99"/>
-      <c r="S36" s="100"/>
+      <c r="B36" s="138"/>
+      <c r="C36" s="139"/>
+      <c r="D36" s="130"/>
+      <c r="E36" s="131"/>
+      <c r="F36" s="131"/>
+      <c r="G36" s="131"/>
+      <c r="H36" s="131"/>
+      <c r="I36" s="131"/>
+      <c r="J36" s="131"/>
+      <c r="K36" s="131"/>
+      <c r="L36" s="131"/>
+      <c r="M36" s="131"/>
+      <c r="N36" s="131"/>
+      <c r="O36" s="131"/>
+      <c r="P36" s="131"/>
+      <c r="Q36" s="131"/>
+      <c r="R36" s="131"/>
+      <c r="S36" s="132"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="106"/>
-      <c r="C37" s="107"/>
-      <c r="D37" s="98"/>
-      <c r="E37" s="99"/>
-      <c r="F37" s="99"/>
-      <c r="G37" s="99"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="99"/>
-      <c r="K37" s="99"/>
-      <c r="L37" s="99"/>
-      <c r="M37" s="99"/>
-      <c r="N37" s="99"/>
-      <c r="O37" s="99"/>
-      <c r="P37" s="99"/>
-      <c r="Q37" s="99"/>
-      <c r="R37" s="99"/>
-      <c r="S37" s="100"/>
+      <c r="B37" s="138"/>
+      <c r="C37" s="139"/>
+      <c r="D37" s="130"/>
+      <c r="E37" s="131"/>
+      <c r="F37" s="131"/>
+      <c r="G37" s="131"/>
+      <c r="H37" s="131"/>
+      <c r="I37" s="131"/>
+      <c r="J37" s="131"/>
+      <c r="K37" s="131"/>
+      <c r="L37" s="131"/>
+      <c r="M37" s="131"/>
+      <c r="N37" s="131"/>
+      <c r="O37" s="131"/>
+      <c r="P37" s="131"/>
+      <c r="Q37" s="131"/>
+      <c r="R37" s="131"/>
+      <c r="S37" s="132"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="108"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="102"/>
-      <c r="F38" s="102"/>
-      <c r="G38" s="102"/>
-      <c r="H38" s="102"/>
-      <c r="I38" s="102"/>
-      <c r="J38" s="102"/>
-      <c r="K38" s="102"/>
-      <c r="L38" s="102"/>
-      <c r="M38" s="102"/>
-      <c r="N38" s="102"/>
-      <c r="O38" s="102"/>
-      <c r="P38" s="102"/>
-      <c r="Q38" s="102"/>
-      <c r="R38" s="102"/>
-      <c r="S38" s="103"/>
+      <c r="B38" s="140"/>
+      <c r="C38" s="141"/>
+      <c r="D38" s="133"/>
+      <c r="E38" s="134"/>
+      <c r="F38" s="134"/>
+      <c r="G38" s="134"/>
+      <c r="H38" s="134"/>
+      <c r="I38" s="134"/>
+      <c r="J38" s="134"/>
+      <c r="K38" s="134"/>
+      <c r="L38" s="134"/>
+      <c r="M38" s="134"/>
+      <c r="N38" s="134"/>
+      <c r="O38" s="134"/>
+      <c r="P38" s="134"/>
+      <c r="Q38" s="134"/>
+      <c r="R38" s="134"/>
+      <c r="S38" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>